<commit_message>
new rates as of 3/18
</commit_message>
<xml_diff>
--- a/db/papacantella.xlsx
+++ b/db/papacantella.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Brookshire, TX</t>
   </si>
@@ -53,13 +53,22 @@
     <t>Morris, IL</t>
   </si>
   <si>
-    <t>Belleville, MI</t>
-  </si>
-  <si>
     <t>Destination</t>
   </si>
   <si>
     <t>Grand Prairie, TX</t>
+  </si>
+  <si>
+    <t>Monroe Township, NJ</t>
+  </si>
+  <si>
+    <t>Monrovia, MD</t>
+  </si>
+  <si>
+    <t>Belleville,  MI</t>
+  </si>
+  <si>
+    <t>Owatonna, MN</t>
   </si>
 </sst>
 </file>
@@ -378,18 +387,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -398,9 +406,9 @@
     <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -444,8 +452,11 @@
       <c r="O1">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -479,50 +490,59 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>249</v>
+        <v>290</v>
       </c>
       <c r="C3" s="1">
-        <v>499</v>
+        <v>570</v>
       </c>
       <c r="D3" s="1">
-        <v>749</v>
+        <v>850</v>
       </c>
       <c r="E3" s="1">
-        <v>999</v>
+        <v>1120</v>
       </c>
       <c r="F3" s="1">
-        <v>1249</v>
+        <v>1400</v>
       </c>
       <c r="G3" s="1">
-        <v>1499</v>
+        <v>1680</v>
       </c>
       <c r="H3" s="1">
-        <v>1574</v>
+        <v>1945</v>
       </c>
       <c r="I3" s="1">
-        <v>1799</v>
+        <v>2200</v>
       </c>
       <c r="J3" s="1">
-        <v>2024</v>
+        <v>2475</v>
       </c>
       <c r="K3" s="1">
-        <v>2099</v>
+        <v>2750</v>
       </c>
       <c r="L3" s="1">
-        <v>2309</v>
+        <v>3000</v>
       </c>
       <c r="M3" s="1">
-        <v>2519</v>
-      </c>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3240</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3510</v>
+      </c>
+      <c r="O3" s="1">
+        <v>3780</v>
+      </c>
+      <c r="P3" s="1">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -568,8 +588,9 @@
       <c r="O4" s="1">
         <v>2750</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -615,51 +636,59 @@
       <c r="O5" s="1">
         <v>1350</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>414</v>
+        <v>465</v>
       </c>
       <c r="C6" s="1">
-        <v>729</v>
+        <v>800</v>
       </c>
       <c r="D6" s="1">
-        <v>1079</v>
+        <v>1185</v>
       </c>
       <c r="E6" s="1">
-        <v>1399</v>
+        <v>1540</v>
       </c>
       <c r="F6" s="1">
-        <v>1596</v>
+        <v>1825</v>
       </c>
       <c r="G6" s="1">
-        <v>1915</v>
+        <v>2160</v>
       </c>
       <c r="H6" s="1">
-        <v>2099</v>
+        <v>2415</v>
       </c>
       <c r="I6" s="1">
-        <v>2399</v>
+        <v>2760</v>
       </c>
       <c r="J6" s="1">
-        <v>2520</v>
+        <v>3060</v>
       </c>
       <c r="K6" s="1">
-        <v>2661</v>
+        <v>3400</v>
       </c>
       <c r="L6" s="1">
-        <v>2928</v>
+        <v>3740</v>
       </c>
       <c r="M6" s="1">
-        <v>3194</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4080</v>
+      </c>
+      <c r="N6" s="1">
+        <v>4355</v>
+      </c>
+      <c r="O6" s="1">
+        <v>4690</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -701,8 +730,9 @@
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -744,8 +774,9 @@
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -791,8 +822,9 @@
       <c r="O9" s="1">
         <v>2200</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -838,8 +870,9 @@
       <c r="O10" s="1">
         <v>1400</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -885,10 +918,11 @@
       <c r="O11" s="1">
         <v>1400</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>400</v>
@@ -899,6 +933,138 @@
       <c r="D12" s="1">
         <v>975</v>
       </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>470</v>
+      </c>
+      <c r="C13" s="1">
+        <v>880</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1245</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1580</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1925</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2280</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2625</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2920</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3240</v>
+      </c>
+      <c r="K13" s="1">
+        <v>3550</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>470</v>
+      </c>
+      <c r="C14" s="1">
+        <v>880</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1245</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1580</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1925</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2280</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2625</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2920</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3240</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3550</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>525</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1135</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1475</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1580</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1840</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2190</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2345</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2600</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2880</v>
+      </c>
+      <c r="K15" s="1">
+        <v>3130</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>